<commit_message>
Updated Subtitle review task
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="181">
   <si>
     <t>Name</t>
   </si>
@@ -555,9 +555,6 @@
     <t>D:\Document Folder\UiPath\Longform_SubtitleReview_Bot\Data\Report.xlsx</t>
   </si>
   <si>
-    <t>Subtitling</t>
-  </si>
-  <si>
     <t>TOONCAST NETWORK</t>
   </si>
   <si>
@@ -573,7 +570,22 @@
     <t>Subtitle_Task_WF Type</t>
   </si>
   <si>
-    <t>2021128-21</t>
+    <t>Sub_MarkerComment</t>
+  </si>
+  <si>
+    <t>Subtitle Marker comment</t>
+  </si>
+  <si>
+    <t>Sub_Rev_Status</t>
+  </si>
+  <si>
+    <t>Approve</t>
+  </si>
+  <si>
+    <t>Subtitle Review</t>
+  </si>
+  <si>
+    <t>147871-177</t>
   </si>
 </sst>
 </file>
@@ -924,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1056,7 +1068,7 @@
         <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1088,7 +1100,7 @@
         <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1565,30 +1577,44 @@
     </row>
     <row r="75" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B75" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B77" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B78" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
     <row r="80" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>